<commit_message>
Updated some tests. Tweaked attendence borders
</commit_message>
<xml_diff>
--- a/demo/demo_empty_workbook.xlsx
+++ b/demo/demo_empty_workbook.xlsx
@@ -57,10 +57,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyBorder="1">
+      <protection locked="1" hidden="false"/>
+    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" applyNumberFormat="1">
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyBorder="1">
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyBorder="1">
@@ -448,8 +448,8 @@
       <c r="C3" s="0" t="str">
         <v>andersol</v>
       </c>
-      <c r="D3" s="0">
-        <v>0</v>
+      <c r="D3" s="0" t="str">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" customFormat="false">
@@ -462,8 +462,8 @@
       <c r="C4" s="0" t="str">
         <v>brownb</v>
       </c>
-      <c r="D4" s="0">
-        <v>0</v>
+      <c r="D4" s="0" t="str">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" customFormat="false">
@@ -476,8 +476,8 @@
       <c r="C5" s="0" t="str">
         <v>davisc</v>
       </c>
-      <c r="D5" s="0">
-        <v>0</v>
+      <c r="D5" s="0" t="str">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" customFormat="false">
@@ -490,8 +490,8 @@
       <c r="C6" s="0" t="str">
         <v>evansa</v>
       </c>
-      <c r="D6" s="0">
-        <v>0</v>
+      <c r="D6" s="0" t="str">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" customFormat="false">
@@ -504,8 +504,8 @@
       <c r="C7" s="0" t="str">
         <v>floresc</v>
       </c>
-      <c r="D7" s="0">
-        <v>0</v>
+      <c r="D7" s="0" t="str">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" customFormat="false">
@@ -518,8 +518,8 @@
       <c r="C8" s="0" t="str">
         <v>garciam</v>
       </c>
-      <c r="D8" s="0">
-        <v>0</v>
+      <c r="D8" s="0" t="str">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" customFormat="false">
@@ -532,8 +532,8 @@
       <c r="C9" s="0" t="str">
         <v>hernandi</v>
       </c>
-      <c r="D9" s="0">
-        <v>0</v>
+      <c r="D9" s="0" t="str">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4" customFormat="false">
@@ -546,8 +546,8 @@
       <c r="C10" s="0" t="str">
         <v>jacksonr</v>
       </c>
-      <c r="D10" s="0">
-        <v>0</v>
+      <c r="D10" s="0" t="str">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" customFormat="false">
@@ -560,8 +560,8 @@
       <c r="C11" s="0" t="str">
         <v>kimj</v>
       </c>
-      <c r="D11" s="0">
-        <v>0</v>
+      <c r="D11" s="0" t="str">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" customFormat="false">
@@ -574,8 +574,8 @@
       <c r="C12" s="0" t="str">
         <v>leee</v>
       </c>
-      <c r="D12" s="0">
-        <v>0</v>
+      <c r="D12" s="0" t="str">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" customFormat="false">
@@ -588,8 +588,8 @@
       <c r="C13" s="0" t="str">
         <v>martinep</v>
       </c>
-      <c r="D13" s="0">
-        <v>0</v>
+      <c r="D13" s="0" t="str">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:4" customFormat="false">
@@ -602,8 +602,8 @@
       <c r="C14" s="0" t="str">
         <v>nelsonm</v>
       </c>
-      <c r="D14" s="0">
-        <v>0</v>
+      <c r="D14" s="0" t="str">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" customFormat="false">
@@ -611,13 +611,13 @@
         <v>Ortiz</v>
       </c>
       <c r="B15" s="0" t="str">
-        <v>Jared</v>
+        <v>Michael</v>
       </c>
       <c r="C15" s="0" t="str">
-        <v>oritzj</v>
-      </c>
-      <c r="D15" s="0">
-        <v>0</v>
+        <v>oritzm</v>
+      </c>
+      <c r="D15" s="0" t="str">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4" customFormat="false">
@@ -630,8 +630,8 @@
       <c r="C16" s="0" t="str">
         <v>patelj</v>
       </c>
-      <c r="D16" s="0">
-        <v>0</v>
+      <c r="D16" s="0" t="str">
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4" customFormat="false">
@@ -644,8 +644,8 @@
       <c r="C17" s="0" t="str">
         <v>quinna</v>
       </c>
-      <c r="D17" s="0">
-        <v>0</v>
+      <c r="D17" s="0" t="str">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2101,91 +2101,91 @@
         <f>info!F2</f>
         <v/>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="4">
         <v>44936.0</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="4">
         <v>44938.0</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="4">
         <v>44943.0</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="4">
         <v>44945.0</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="4">
         <v>44952.0</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="4">
         <v>44957.0</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="4">
         <v>44959.0</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="4">
         <v>44964.0</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="4">
         <v>44966.0</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="4">
         <v>44971.0</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q2" s="4">
         <v>44973.0</v>
       </c>
-      <c r="R2" s="3">
+      <c r="R2" s="4">
         <v>44978.0</v>
       </c>
-      <c r="S2" s="3">
+      <c r="S2" s="4">
         <v>44980.0</v>
       </c>
-      <c r="T2" s="3">
+      <c r="T2" s="4">
         <v>44985.0</v>
       </c>
-      <c r="U2" s="3">
+      <c r="U2" s="4">
         <v>44987.0</v>
       </c>
-      <c r="V2" s="3">
+      <c r="V2" s="4">
         <v>44999.0</v>
       </c>
-      <c r="W2" s="3">
+      <c r="W2" s="4">
         <v>45001.0</v>
       </c>
-      <c r="X2" s="3">
+      <c r="X2" s="4">
         <v>45006.0</v>
       </c>
-      <c r="Y2" s="3">
+      <c r="Y2" s="4">
         <v>45008.0</v>
       </c>
-      <c r="Z2" s="3">
+      <c r="Z2" s="4">
         <v>45013.0</v>
       </c>
-      <c r="AA2" s="3">
+      <c r="AA2" s="4">
         <v>45015.0</v>
       </c>
-      <c r="AB2" s="3">
+      <c r="AB2" s="4">
         <v>45020.0</v>
       </c>
-      <c r="AC2" s="3">
+      <c r="AC2" s="4">
         <v>45022.0</v>
       </c>
-      <c r="AD2" s="3">
+      <c r="AD2" s="4">
         <v>45027.0</v>
       </c>
-      <c r="AE2" s="3">
+      <c r="AE2" s="4">
         <v>45029.0</v>
       </c>
-      <c r="AF2" s="3">
+      <c r="AF2" s="4">
         <v>45034.0</v>
       </c>
-      <c r="AG2" s="3">
+      <c r="AG2" s="4">
         <v>45036.0</v>
       </c>
-      <c r="AH2" s="3">
+      <c r="AH2" s="4">
         <v>45041.0</v>
       </c>
-      <c r="AI2" s="3">
+      <c r="AI2" s="4">
         <v>45043.0</v>
       </c>
     </row>
@@ -2214,7 +2214,7 @@
         <f>info!F3</f>
         <v/>
       </c>
-      <c r="G3" s="2" t="str">
+      <c r="G3" s="5" t="str">
         <v/>
       </c>
       <c r="H3" s="5" t="str">
@@ -2303,31 +2303,31 @@
       </c>
     </row>
     <row r="4" spans="1:35" customFormat="false">
-      <c r="A4" s="1">
+      <c r="A4" s="3">
         <f>info!A4</f>
         <v/>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <f>info!B4</f>
         <v/>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <f>info!C4</f>
         <v/>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="3">
         <f>info!D4</f>
         <v/>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="3">
         <f>info!E4</f>
         <v/>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="3">
         <f>info!F4</f>
         <v/>
       </c>
-      <c r="G4" s="4" t="str">
+      <c r="G4" s="6" t="str">
         <v/>
       </c>
       <c r="H4" s="6" t="str">
@@ -2416,31 +2416,31 @@
       </c>
     </row>
     <row r="5" spans="1:35" customFormat="false">
-      <c r="A5" s="1">
+      <c r="A5" s="3">
         <f>info!A5</f>
         <v/>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3">
         <f>info!B5</f>
         <v/>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <f>info!C5</f>
         <v/>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="3">
         <f>info!D5</f>
         <v/>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="3">
         <f>info!E5</f>
         <v/>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="3">
         <f>info!F5</f>
         <v/>
       </c>
-      <c r="G5" s="4" t="str">
+      <c r="G5" s="6" t="str">
         <v/>
       </c>
       <c r="H5" s="6" t="str">
@@ -2529,31 +2529,31 @@
       </c>
     </row>
     <row r="6" spans="1:35" customFormat="false">
-      <c r="A6" s="1">
+      <c r="A6" s="3">
         <f>info!A6</f>
         <v/>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="3">
         <f>info!B6</f>
         <v/>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <f>info!C6</f>
         <v/>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="3">
         <f>info!D6</f>
         <v/>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="3">
         <f>info!E6</f>
         <v/>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="3">
         <f>info!F6</f>
         <v/>
       </c>
-      <c r="G6" s="4" t="str">
+      <c r="G6" s="6" t="str">
         <v/>
       </c>
       <c r="H6" s="6" t="str">
@@ -2642,31 +2642,31 @@
       </c>
     </row>
     <row r="7" spans="1:35" customFormat="false">
-      <c r="A7" s="1">
+      <c r="A7" s="3">
         <f>info!A7</f>
         <v/>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="3">
         <f>info!B7</f>
         <v/>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <f>info!C7</f>
         <v/>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="3">
         <f>info!D7</f>
         <v/>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="3">
         <f>info!E7</f>
         <v/>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="3">
         <f>info!F7</f>
         <v/>
       </c>
-      <c r="G7" s="4" t="str">
+      <c r="G7" s="6" t="str">
         <v/>
       </c>
       <c r="H7" s="6" t="str">
@@ -2755,31 +2755,31 @@
       </c>
     </row>
     <row r="8" spans="1:35" customFormat="false">
-      <c r="A8" s="1">
+      <c r="A8" s="3">
         <f>info!A8</f>
         <v/>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="3">
         <f>info!B8</f>
         <v/>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <f>info!C8</f>
         <v/>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="3">
         <f>info!D8</f>
         <v/>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="3">
         <f>info!E8</f>
         <v/>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="3">
         <f>info!F8</f>
         <v/>
       </c>
-      <c r="G8" s="4" t="str">
+      <c r="G8" s="6" t="str">
         <v/>
       </c>
       <c r="H8" s="6" t="str">
@@ -2868,31 +2868,31 @@
       </c>
     </row>
     <row r="9" spans="1:35" customFormat="false">
-      <c r="A9" s="1">
+      <c r="A9" s="3">
         <f>info!A9</f>
         <v/>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="3">
         <f>info!B9</f>
         <v/>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <f>info!C9</f>
         <v/>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="3">
         <f>info!D9</f>
         <v/>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="3">
         <f>info!E9</f>
         <v/>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="3">
         <f>info!F9</f>
         <v/>
       </c>
-      <c r="G9" s="4" t="str">
+      <c r="G9" s="6" t="str">
         <v/>
       </c>
       <c r="H9" s="6" t="str">
@@ -2981,31 +2981,31 @@
       </c>
     </row>
     <row r="10" spans="1:35" customFormat="false">
-      <c r="A10" s="1">
+      <c r="A10" s="3">
         <f>info!A10</f>
         <v/>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="3">
         <f>info!B10</f>
         <v/>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <f>info!C10</f>
         <v/>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="3">
         <f>info!D10</f>
         <v/>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="3">
         <f>info!E10</f>
         <v/>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="3">
         <f>info!F10</f>
         <v/>
       </c>
-      <c r="G10" s="4" t="str">
+      <c r="G10" s="6" t="str">
         <v/>
       </c>
       <c r="H10" s="6" t="str">
@@ -3094,31 +3094,31 @@
       </c>
     </row>
     <row r="11" spans="1:35" customFormat="false">
-      <c r="A11" s="1">
+      <c r="A11" s="3">
         <f>info!A11</f>
         <v/>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="3">
         <f>info!B11</f>
         <v/>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="3">
         <f>info!C11</f>
         <v/>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="3">
         <f>info!D11</f>
         <v/>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="3">
         <f>info!E11</f>
         <v/>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="3">
         <f>info!F11</f>
         <v/>
       </c>
-      <c r="G11" s="4" t="str">
+      <c r="G11" s="6" t="str">
         <v/>
       </c>
       <c r="H11" s="6" t="str">
@@ -3207,31 +3207,31 @@
       </c>
     </row>
     <row r="12" spans="1:35" customFormat="false">
-      <c r="A12" s="1">
+      <c r="A12" s="3">
         <f>info!A12</f>
         <v/>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="3">
         <f>info!B12</f>
         <v/>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="3">
         <f>info!C12</f>
         <v/>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="3">
         <f>info!D12</f>
         <v/>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="3">
         <f>info!E12</f>
         <v/>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="3">
         <f>info!F12</f>
         <v/>
       </c>
-      <c r="G12" s="4" t="str">
+      <c r="G12" s="6" t="str">
         <v/>
       </c>
       <c r="H12" s="6" t="str">
@@ -3320,31 +3320,31 @@
       </c>
     </row>
     <row r="13" spans="1:35" customFormat="false">
-      <c r="A13" s="1">
+      <c r="A13" s="3">
         <f>info!A13</f>
         <v/>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="3">
         <f>info!B13</f>
         <v/>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="3">
         <f>info!C13</f>
         <v/>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="3">
         <f>info!D13</f>
         <v/>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="3">
         <f>info!E13</f>
         <v/>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="3">
         <f>info!F13</f>
         <v/>
       </c>
-      <c r="G13" s="4" t="str">
+      <c r="G13" s="6" t="str">
         <v/>
       </c>
       <c r="H13" s="6" t="str">
@@ -3433,31 +3433,31 @@
       </c>
     </row>
     <row r="14" spans="1:35" customFormat="false">
-      <c r="A14" s="1">
+      <c r="A14" s="3">
         <f>info!A14</f>
         <v/>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="3">
         <f>info!B14</f>
         <v/>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="3">
         <f>info!C14</f>
         <v/>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="3">
         <f>info!D14</f>
         <v/>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="3">
         <f>info!E14</f>
         <v/>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="3">
         <f>info!F14</f>
         <v/>
       </c>
-      <c r="G14" s="4" t="str">
+      <c r="G14" s="6" t="str">
         <v/>
       </c>
       <c r="H14" s="6" t="str">
@@ -3546,31 +3546,31 @@
       </c>
     </row>
     <row r="15" spans="1:35" customFormat="false">
-      <c r="A15" s="1">
+      <c r="A15" s="3">
         <f>info!A15</f>
         <v/>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="3">
         <f>info!B15</f>
         <v/>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="3">
         <f>info!C15</f>
         <v/>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="3">
         <f>info!D15</f>
         <v/>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="3">
         <f>info!E15</f>
         <v/>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="3">
         <f>info!F15</f>
         <v/>
       </c>
-      <c r="G15" s="4" t="str">
+      <c r="G15" s="6" t="str">
         <v/>
       </c>
       <c r="H15" s="6" t="str">
@@ -3659,31 +3659,31 @@
       </c>
     </row>
     <row r="16" spans="1:35" customFormat="false">
-      <c r="A16" s="1">
+      <c r="A16" s="3">
         <f>info!A16</f>
         <v/>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="3">
         <f>info!B16</f>
         <v/>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="3">
         <f>info!C16</f>
         <v/>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="3">
         <f>info!D16</f>
         <v/>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="3">
         <f>info!E16</f>
         <v/>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="3">
         <f>info!F16</f>
         <v/>
       </c>
-      <c r="G16" s="4" t="str">
+      <c r="G16" s="6" t="str">
         <v/>
       </c>
       <c r="H16" s="6" t="str">
@@ -3772,31 +3772,31 @@
       </c>
     </row>
     <row r="17" spans="1:35" customFormat="false">
-      <c r="A17" s="1">
+      <c r="A17" s="3">
         <f>info!A17</f>
         <v/>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="3">
         <f>info!B17</f>
         <v/>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="3">
         <f>info!C17</f>
         <v/>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="3">
         <f>info!D17</f>
         <v/>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="3">
         <f>info!E17</f>
         <v/>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="3">
         <f>info!F17</f>
         <v/>
       </c>
-      <c r="G17" s="4" t="str">
+      <c r="G17" s="6" t="str">
         <v/>
       </c>
       <c r="H17" s="6" t="str">

</xml_diff>